<commit_message>
Addressed PR comments and fixed some bugs
</commit_message>
<xml_diff>
--- a/src/mappings/ics/xlsx/veris-1_3_7-mappings-ics_v12.xlsx
+++ b/src/mappings/ics/xlsx/veris-1_3_7-mappings-ics_v12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitre-my.sharepoint.com/personal/javoss_mitre_org/Documents/Documents/Veris II/veris-2/src/mappings/ics/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbergeron\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{6EEF743F-5A67-4095-9381-1DC2EF84ECD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBCD1107-B0CF-42A8-9DE9-0CB7321D594A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8CCF4E-CF1F-4F58-A8AB-3AD9DD10045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="11" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
+    <workbookView xWindow="-25320" yWindow="405" windowWidth="25440" windowHeight="15390" firstSheet="3" activeTab="4" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="416">
   <si>
     <t>ATT&amp;CK Integration into VERIS</t>
   </si>
@@ -2597,7 +2597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B670464-1153-4AA6-978E-5B7FAB2C4B98}">
   <dimension ref="A1:C770"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -8609,10 +8609,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDB77F8-08D1-470F-BA2C-78FD3244C97D}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C11"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8676,49 +8676,6 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B11" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{BE1002AF-9085-461D-9027-25BC22637C47}"/>
@@ -8726,23 +8683,18 @@
     <hyperlink ref="B4" r:id="rId3" display="https://attack.mitre.org/techniques/T0859" xr:uid="{402347B8-ACB8-400E-A471-DF1E9F5E2888}"/>
     <hyperlink ref="B5" r:id="rId4" display="https://attack.mitre.org/techniques/T0882" xr:uid="{8B33FEBA-4C72-4B92-B046-CE68725D749E}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{7DF776B2-230A-42DD-9E69-2A6582CD126F}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{4F0EB2DE-82BD-4BE3-B69D-0CD283D7A24A}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{2753AC4A-448D-4ED1-B43A-42380FD44D0C}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{34E53570-F479-48D6-9C1F-F69988C5AC68}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{1710B428-C825-4560-9640-0ED86A244E3F}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{BA781074-89A4-4B27-B177-BE0D3AB0F999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0720A71-FEE1-42C9-B26A-BF04E4E8C788}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8931,43 +8883,83 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="B21" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B25" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="19"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="19"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="19"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="19"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B28" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="19"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8977,7 +8969,7 @@
     <hyperlink ref="B4" r:id="rId4" display="https://attack.mitre.org/techniques/T0805" xr:uid="{F3034DBB-E459-D74F-88A6-750589CC67CF}"/>
     <hyperlink ref="B5" r:id="rId5" display="https://attack.mitre.org/techniques/T0858" xr:uid="{4BAD9B53-CB8E-E744-A137-42AD6CE6F07B}"/>
     <hyperlink ref="B12" r:id="rId6" display="https://attack.mitre.org/techniques/T0872" xr:uid="{DFA39C3F-1271-C245-A02B-A0D28D86D385}"/>
-    <hyperlink ref="B23" r:id="rId7" display="https://attack.mitre.org/techniques/T0867" xr:uid="{5648B64F-9B71-B745-BFC0-F93652EB1F9A}"/>
+    <hyperlink ref="B28" r:id="rId7" display="https://attack.mitre.org/techniques/T0867" xr:uid="{5648B64F-9B71-B745-BFC0-F93652EB1F9A}"/>
     <hyperlink ref="B11" r:id="rId8" display="https://attack.mitre.org/techniques/T0862" xr:uid="{F85A74BF-9DE7-1B4F-A2EC-381EF502B332}"/>
     <hyperlink ref="B13" r:id="rId9" display="https://attack.mitre.org/techniques/T0856" xr:uid="{4650DE3B-7840-3E4A-80D1-9BEAD9B90089}"/>
     <hyperlink ref="B19" r:id="rId10" display="https://attack.mitre.org/techniques/T0856" xr:uid="{A2A15B08-F6EA-DA44-ACCB-F682A1B39351}"/>
@@ -8987,9 +8979,14 @@
     <hyperlink ref="B17" r:id="rId14" xr:uid="{F3A7E00E-F3FF-4D04-B057-BD56A302C89E}"/>
     <hyperlink ref="B16" r:id="rId15" xr:uid="{8A78A68C-23BB-43A7-AA80-3DD9C8AF0B56}"/>
     <hyperlink ref="B14" r:id="rId16" xr:uid="{9984584F-DEBD-4CD7-8718-40B885F82E70}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{4F0EB2DE-82BD-4BE3-B69D-0CD283D7A24A}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{2753AC4A-448D-4ED1-B43A-42380FD44D0C}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{34E53570-F479-48D6-9C1F-F69988C5AC68}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{1710B428-C825-4560-9640-0ED86A244E3F}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{BA781074-89A4-4B27-B177-BE0D3AB0F999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -10849,6 +10846,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010052D8A6B6F9FE2E45B0EDBAAD5FAF1312" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7022bf91ca57a9626808ed15fdcbfbd6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xmlns:ns3="ec3e3de1-934b-464b-893a-587ae869df79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d11a2dadb3f3bef5d5d1fdbc6ca57c91" ns2:_="" ns3:_="">
     <xsd:import namespace="0ca01121-da18-407e-86a0-e0ab1b6c7d8c"/>
@@ -11147,15 +11153,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34220A23-D68F-4415-8317-3103A802156C}">
   <ds:schemaRefs>
@@ -11168,6 +11165,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF2F0EC-3847-4FE7-B08A-EEF35C79D6DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96E29817-E7D0-44AC-B47E-87D4D909CCAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11184,12 +11189,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF2F0EC-3847-4FE7-B08A-EEF35C79D6DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Removed old xlsx files and updated value in ics spreadsheet
</commit_message>
<xml_diff>
--- a/src/mappings/ics/xlsx/veris-1_3_7-mappings-ics_v12.xlsx
+++ b/src/mappings/ics/xlsx/veris-1_3_7-mappings-ics_v12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbergeron\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitre-my.sharepoint.com/personal/javoss_mitre_org/Documents/Documents/Veris II/veris-2/src/mappings/ics/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8CCF4E-CF1F-4F58-A8AB-3AD9DD10045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4E8CCF4E-CF1F-4F58-A8AB-3AD9DD10045D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0FBFF53-9F8D-4AFE-88A2-ED5A549BFC4A}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="405" windowWidth="25440" windowHeight="15390" firstSheet="3" activeTab="4" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{698518E7-B140-7645-B530-A1A72BD96EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="416">
   <si>
     <t>ATT&amp;CK Integration into VERIS</t>
   </si>
@@ -8691,10 +8691,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0720A71-FEE1-42C9-B26A-BF04E4E8C788}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8908,58 +8908,50 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B24" s="11" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>168</v>
-      </c>
+      <c r="A25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="19"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="19"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>185</v>
-      </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="19"/>
+        <v>186</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>186</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="19"/>
+      <c r="C29" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8969,7 +8961,7 @@
     <hyperlink ref="B4" r:id="rId4" display="https://attack.mitre.org/techniques/T0805" xr:uid="{F3034DBB-E459-D74F-88A6-750589CC67CF}"/>
     <hyperlink ref="B5" r:id="rId5" display="https://attack.mitre.org/techniques/T0858" xr:uid="{4BAD9B53-CB8E-E744-A137-42AD6CE6F07B}"/>
     <hyperlink ref="B12" r:id="rId6" display="https://attack.mitre.org/techniques/T0872" xr:uid="{DFA39C3F-1271-C245-A02B-A0D28D86D385}"/>
-    <hyperlink ref="B28" r:id="rId7" display="https://attack.mitre.org/techniques/T0867" xr:uid="{5648B64F-9B71-B745-BFC0-F93652EB1F9A}"/>
+    <hyperlink ref="B27" r:id="rId7" display="https://attack.mitre.org/techniques/T0867" xr:uid="{5648B64F-9B71-B745-BFC0-F93652EB1F9A}"/>
     <hyperlink ref="B11" r:id="rId8" display="https://attack.mitre.org/techniques/T0862" xr:uid="{F85A74BF-9DE7-1B4F-A2EC-381EF502B332}"/>
     <hyperlink ref="B13" r:id="rId9" display="https://attack.mitre.org/techniques/T0856" xr:uid="{4650DE3B-7840-3E4A-80D1-9BEAD9B90089}"/>
     <hyperlink ref="B19" r:id="rId10" display="https://attack.mitre.org/techniques/T0856" xr:uid="{A2A15B08-F6EA-DA44-ACCB-F682A1B39351}"/>
@@ -8982,11 +8974,10 @@
     <hyperlink ref="B21" r:id="rId17" xr:uid="{4F0EB2DE-82BD-4BE3-B69D-0CD283D7A24A}"/>
     <hyperlink ref="B22" r:id="rId18" xr:uid="{2753AC4A-448D-4ED1-B43A-42380FD44D0C}"/>
     <hyperlink ref="B23" r:id="rId19" xr:uid="{34E53570-F479-48D6-9C1F-F69988C5AC68}"/>
-    <hyperlink ref="B24" r:id="rId20" xr:uid="{1710B428-C825-4560-9640-0ED86A244E3F}"/>
-    <hyperlink ref="B25" r:id="rId21" xr:uid="{BA781074-89A4-4B27-B177-BE0D3AB0F999}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{BA781074-89A4-4B27-B177-BE0D3AB0F999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -10846,15 +10837,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010052D8A6B6F9FE2E45B0EDBAAD5FAF1312" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7022bf91ca57a9626808ed15fdcbfbd6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0ca01121-da18-407e-86a0-e0ab1b6c7d8c" xmlns:ns3="ec3e3de1-934b-464b-893a-587ae869df79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d11a2dadb3f3bef5d5d1fdbc6ca57c91" ns2:_="" ns3:_="">
     <xsd:import namespace="0ca01121-da18-407e-86a0-e0ab1b6c7d8c"/>
@@ -11153,6 +11135,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34220A23-D68F-4415-8317-3103A802156C}">
   <ds:schemaRefs>
@@ -11165,14 +11156,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF2F0EC-3847-4FE7-B08A-EEF35C79D6DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96E29817-E7D0-44AC-B47E-87D4D909CCAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11189,4 +11172,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF2F0EC-3847-4FE7-B08A-EEF35C79D6DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>